<commit_message>
target function and limits
</commit_message>
<xml_diff>
--- a/Inputdata.xlsx
+++ b/Inputdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Fabian\Code\hydro_opt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF47514D-F5DD-4C19-9A25-58FEC6783A71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{245F6EF1-D0A2-4460-8CBF-F6B65BD14F61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Land</t>
   </si>
@@ -67,6 +67,15 @@
   </si>
   <si>
     <t>CH3OH Schiff Preis</t>
+  </si>
+  <si>
+    <t>H2 Export Limit</t>
+  </si>
+  <si>
+    <t>NH3 Export Limit</t>
+  </si>
+  <si>
+    <t>CH3OH Export Limit</t>
   </si>
 </sst>
 </file>
@@ -384,10 +393,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -395,15 +404,18 @@
     <col min="2" max="2" width="19.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="18.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -417,25 +429,34 @@
         <v>7</v>
       </c>
       <c r="E1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" t="s">
         <v>8</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>9</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>10</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J1" t="s">
         <v>11</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>12</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>13</v>
       </c>
+      <c r="M1" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -449,25 +470,34 @@
         <v>3</v>
       </c>
       <c r="E2">
+        <v>3</v>
+      </c>
+      <c r="F2">
         <v>8</v>
       </c>
-      <c r="F2">
-        <v>4</v>
-      </c>
       <c r="G2">
+        <v>4</v>
+      </c>
+      <c r="H2">
         <v>5</v>
       </c>
-      <c r="H2">
+      <c r="I2">
+        <v>5</v>
+      </c>
+      <c r="J2">
         <v>12</v>
       </c>
-      <c r="I2">
+      <c r="K2">
         <v>6</v>
       </c>
-      <c r="J2">
+      <c r="L2">
         <v>7</v>
       </c>
+      <c r="M2">
+        <v>8</v>
+      </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -481,25 +511,34 @@
         <v>3</v>
       </c>
       <c r="E3">
+        <v>4</v>
+      </c>
+      <c r="F3">
         <v>9</v>
       </c>
-      <c r="F3">
-        <v>4</v>
-      </c>
       <c r="G3">
+        <v>4</v>
+      </c>
+      <c r="H3">
         <v>5</v>
-      </c>
-      <c r="H3">
-        <v>13</v>
       </c>
       <c r="I3">
         <v>6</v>
       </c>
       <c r="J3">
+        <v>13</v>
+      </c>
+      <c r="K3">
+        <v>6</v>
+      </c>
+      <c r="L3">
         <v>7</v>
       </c>
+      <c r="M3">
+        <v>1</v>
+      </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -513,25 +552,34 @@
         <v>3</v>
       </c>
       <c r="E4">
+        <v>5</v>
+      </c>
+      <c r="F4">
         <v>10</v>
       </c>
-      <c r="F4">
-        <v>4</v>
-      </c>
       <c r="G4">
+        <v>4</v>
+      </c>
+      <c r="H4">
         <v>5</v>
       </c>
-      <c r="H4">
+      <c r="I4">
+        <v>2</v>
+      </c>
+      <c r="J4">
         <v>14</v>
       </c>
-      <c r="I4">
+      <c r="K4">
         <v>6</v>
       </c>
-      <c r="J4">
+      <c r="L4">
         <v>7</v>
       </c>
+      <c r="M4">
+        <v>3</v>
+      </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -545,22 +593,31 @@
         <v>9999</v>
       </c>
       <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
         <v>11</v>
-      </c>
-      <c r="F5">
-        <v>0</v>
       </c>
       <c r="G5">
         <v>0</v>
       </c>
       <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>4</v>
+      </c>
+      <c r="J5">
         <v>15</v>
       </c>
-      <c r="I5">
+      <c r="K5">
         <v>0</v>
       </c>
-      <c r="J5">
+      <c r="L5">
         <v>0</v>
+      </c>
+      <c r="M5">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>